<commit_message>
implements import excel data to JTable
</commit_message>
<xml_diff>
--- a/src/main/java/excelFiles/Output.xlsx
+++ b/src/main/java/excelFiles/Output.xlsx
@@ -12,7 +12,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+  <si>
+    <t>编号</t>
+  </si>
+  <si>
+    <t>位置</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>M2 IP</t>
+  </si>
+  <si>
+    <t>M5_Ap IP</t>
+  </si>
+  <si>
+    <t>M5_AP 频率</t>
+  </si>
+  <si>
+    <t>M5_AP mac地址</t>
+  </si>
+  <si>
+    <t>M5_ST IP</t>
+  </si>
+  <si>
+    <t>M5_ST 锁定mac地址</t>
+  </si>
   <si>
     <t>1</t>
   </si>
@@ -21,6 +48,15 @@
   </si>
   <si>
     <t>a + b</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>c + d</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -65,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -81,6 +117,69 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>